<commit_message>
added dynamic pts density signal
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\SignalGenerationConfigs\DynamicPointsDensitySignalConfigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF33C27-AA61-48F6-BA16-854FFE38DEB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5A4A77-0FB7-4660-8A0D-C8C9EAC362A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,10 +54,10 @@
     <t>End Time</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>Points Density</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,7 +431,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>8</v>
@@ -439,34 +439,34 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>150</v>
+        <v>5.5</v>
       </c>
       <c r="C2">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>300</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>300</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="H2">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>500</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
finished TODO for STOP in FrequencySettingModule
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\SignalGenerationConfigs\DynamicPointsDensitySignalConfigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B42F145-FE24-465F-BE65-6AC637DB96E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F480BA9-1752-4197-98ED-E292194662E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,10 +57,10 @@
     <t>Points Density</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>MyConfig</t>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Debug</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,7 +442,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>5.5</v>
@@ -474,25 +474,25 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -501,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debugged start_x, plateau and end_x
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\SignalGenerationConfigs\DynamicPointsDensitySignalConfigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F480BA9-1752-4197-98ED-E292194662E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA10051-A451-4099-9898-FE8E4272BC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-708" yWindow="2952" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,8 +391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,22 +445,22 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -469,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
debug for extreme cases (triangle, meander)
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\SignalGenerationConfigs\DynamicPointsDensitySignalConfigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA10051-A451-4099-9898-FE8E4272BC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88591207-2996-4529-B617-3B75D1202184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-708" yWindow="2952" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Start Time</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Debug</t>
+  </si>
+  <si>
+    <t>Zero</t>
+  </si>
+  <si>
+    <t>ZeroAcc</t>
   </si>
 </sst>
 </file>
@@ -389,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,6 +510,70 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>40</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>40</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added example signals in excel
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\SignalGenerationConfigs\DynamicPointsDensitySignalConfigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88591207-2996-4529-B617-3B75D1202184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C685133-16FB-4FA4-A9CC-923C274E7DB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Start Time</t>
   </si>
@@ -66,7 +66,13 @@
     <t>Zero</t>
   </si>
   <si>
-    <t>ZeroAcc</t>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>Meander</t>
+  </si>
+  <si>
+    <t>Spike</t>
   </si>
 </sst>
 </file>
@@ -395,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,47 +516,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>40</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-    </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -572,6 +546,102 @@
       </c>
       <c r="J5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.02</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>0.02</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0.02</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.02</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pop up window before saving. Saving does not work
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\SignalGenerationConfigs\DynamicPointsDensitySignalConfigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4689C1-E54F-49D4-87F3-C46598250465}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C83B75-4A6D-4F4A-9719-97D60B3E5734}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1176" yWindow="4500" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-468" yWindow="3432" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Start Time</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>High Level Frequency</t>
-  </si>
-  <si>
-    <t>Vertical Offset</t>
   </si>
   <si>
     <t>End Time</t>
@@ -404,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H1" sqref="H1:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,7 +420,7 @@
     <col min="9" max="9" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -446,18 +443,15 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -478,18 +472,15 @@
         <v>40</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -510,18 +501,15 @@
         <v>40</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -542,50 +530,44 @@
         <v>40</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>13</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -606,18 +588,15 @@
         <v>10</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -638,18 +617,15 @@
         <v>10</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -670,12 +646,9 @@
         <v>19.2</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="I10">
-        <v>0.36</v>
-      </c>
-      <c r="J10">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WORKS preset save & auto fill. BUT buggy preset deletion with push button
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
@@ -576,17 +576,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19.64</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>60.01</v>
+        <v>22.92</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>8</v>
@@ -607,7 +607,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -620,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>43.64333333333333</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1.38</v>
       </c>
       <c r="G6" t="n">
         <v>50</v>

</xml_diff>

<commit_message>
now Request freq is in excel configs
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/SignalConfigs.xlsx
@@ -1,43 +1,93 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\SignalGenerationConfigs\DynamicPointsDensitySignalConfigs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A457A29-9903-431D-9110-967892214DA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Config Name</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>Acceleration Time</t>
+  </si>
+  <si>
+    <t>Plateau Time</t>
+  </si>
+  <si>
+    <t>Deceleration Time</t>
+  </si>
+  <si>
+    <t>Low Level Frequency</t>
+  </si>
+  <si>
+    <t>High Level Frequency</t>
+  </si>
+  <si>
+    <t>Points Density</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Request Frequency</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -46,93 +96,57 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,219 +434,141 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Config Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Acceleration Time</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Plateau Time</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Deceleration Time</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Low Level Frequency</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>High Level Frequency</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Points Density</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Debug</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" t="n">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
         <v>5</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>20</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>6</v>
       </c>
+      <c r="J2">
+        <v>0.9</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>20</v>
       </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
         <v>20</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>20</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" t="n">
-        <v>3</v>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>0.9</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Fast</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="n">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>8</v>
       </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>8</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>50</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="n">
-        <v>22.92</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>50</v>
-      </c>
-      <c r="H5" t="n">
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
         <v>1</v>
-      </c>
-      <c r="I5" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" t="n">
-        <v>22.92</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>43.64333333333333</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="G6" t="n">
-        <v>50</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>